<commit_message>
fix api thêm lớp = excel với chuongtrinhdaotao mới
</commit_message>
<xml_diff>
--- a/Tài liệu/lop_data.xlsx
+++ b/Tài liệu/lop_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\NghienCuuKhoaHoc\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BE7801-B675-4D55-A014-8E1FBD96BAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB7B567-0E36-4577-AC3E-39E57133E96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>MALOP</t>
   </si>
@@ -57,9 +57,6 @@
     <t>DA32TTF</t>
   </si>
   <si>
-    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2020</t>
-  </si>
-  <si>
     <t>công nghệ thông tin A</t>
   </si>
   <si>
@@ -81,10 +78,25 @@
     <t>Bộ môn Công nghệ thông tin</t>
   </si>
   <si>
-    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2027</t>
-  </si>
-  <si>
-    <t>CÔNG NGHỆ THÔNG TIN KHÓA 2028</t>
+    <t>SO_QUYET_DINH</t>
+  </si>
+  <si>
+    <t>TRINH_DO</t>
+  </si>
+  <si>
+    <t>TONG_SO_TIN_CHI</t>
+  </si>
+  <si>
+    <t>MO_TA_HOC_KY</t>
+  </si>
+  <si>
+    <t>3455/QĐ-ĐHTV, ngày 12 tháng 7 năm 2018</t>
+  </si>
+  <si>
+    <t>ĐẠI HỌC</t>
+  </si>
+  <si>
+    <t>CÔNG NGHỆ THÔNG TIN</t>
   </si>
 </sst>
 </file>
@@ -126,9 +138,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -409,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,127 +438,215 @@
     <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1">
+        <v>138</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>2021</v>
-      </c>
-      <c r="E2">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E3" s="1">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1">
+        <v>138</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>2024</v>
-      </c>
-      <c r="E3">
+      <c r="D4" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E4" s="1">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1">
+        <v>138</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>2022</v>
-      </c>
-      <c r="E4">
+      <c r="D5" s="1">
+        <v>2025</v>
+      </c>
+      <c r="E5" s="1">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <v>138</v>
+      </c>
+      <c r="J5" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>2025</v>
-      </c>
-      <c r="E5">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>2023</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>44</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1">
+        <v>138</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update file excel lop
</commit_message>
<xml_diff>
--- a/Tài liệu/lop_data.xlsx
+++ b/Tài liệu/lop_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\NghienCuuKhoaHoc\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB7B567-0E36-4577-AC3E-39E57133E96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8205771F-A5EF-4156-80B1-5F2E58D3CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
   <si>
     <t>MALOP</t>
   </si>
@@ -54,24 +54,6 @@
     <t>DA24TTD</t>
   </si>
   <si>
-    <t>DA32TTF</t>
-  </si>
-  <si>
-    <t>công nghệ thông tin A</t>
-  </si>
-  <si>
-    <t>công nghệ thông tin B</t>
-  </si>
-  <si>
-    <t>công nghệ thông tin C</t>
-  </si>
-  <si>
-    <t>công nghệ thông tin E</t>
-  </si>
-  <si>
-    <t>công nghệ thông tin F</t>
-  </si>
-  <si>
     <t>TENBOMON</t>
   </si>
   <si>
@@ -97,13 +79,103 @@
   </si>
   <si>
     <t>CÔNG NGHỆ THÔNG TIN</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin A 2020</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin B 2020</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin A 2021</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin B 2021</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin C 2021</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin A 2022</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin B 2022</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin C 2022</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin D 2022</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin A 2023</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin B 2023</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin C 2023</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin D 2023</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin A 2024</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin B 2024</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin C 2024</t>
+  </si>
+  <si>
+    <t>Đại học Công nghệ thông tin D 2024</t>
+  </si>
+  <si>
+    <t>DA20TTA</t>
+  </si>
+  <si>
+    <t>DA20TTB</t>
+  </si>
+  <si>
+    <t>DA21TTB</t>
+  </si>
+  <si>
+    <t>DA21TTC</t>
+  </si>
+  <si>
+    <t>DA22TTA</t>
+  </si>
+  <si>
+    <t>DA22TTC</t>
+  </si>
+  <si>
+    <t>DA22TTD</t>
+  </si>
+  <si>
+    <t>DA23TTA</t>
+  </si>
+  <si>
+    <t>DA23TTB</t>
+  </si>
+  <si>
+    <t>DA23TTD</t>
+  </si>
+  <si>
+    <t>DA24TTA</t>
+  </si>
+  <si>
+    <t>DA24TTB</t>
+  </si>
+  <si>
+    <t>DA24TTC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +189,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -126,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,17 +219,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -426,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +550,7 @@
     <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,194 +567,567 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E2" s="4">
+        <v>30</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1">
+        <v>138</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="D3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="4">
+        <v>44</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1">
+        <v>138</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="D4" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E4" s="4">
+        <v>44</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1">
+        <v>138</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E5" s="4">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1">
+        <v>138</v>
+      </c>
+      <c r="J5" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2021</v>
+      </c>
+      <c r="E6" s="4">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="1">
+        <v>138</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2021</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="D7" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E7" s="4">
+        <v>50</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1">
+        <v>138</v>
+      </c>
+      <c r="J7" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E8" s="4">
+        <v>47</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1">
+        <v>138</v>
+      </c>
+      <c r="J8" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1">
-        <v>138</v>
-      </c>
-      <c r="J2" s="1">
-        <v>7480201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E9" s="4">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1">
+        <v>138</v>
+      </c>
+      <c r="J9" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E10" s="4">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>138</v>
+      </c>
+      <c r="J10" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E11" s="4">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1">
+        <v>138</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E12" s="4">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1">
+        <v>138</v>
+      </c>
+      <c r="J12" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E13" s="4">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="1">
+        <v>138</v>
+      </c>
+      <c r="J13" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2023</v>
+      </c>
+      <c r="E14" s="4">
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="1">
+        <v>138</v>
+      </c>
+      <c r="J14" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1">
         <v>2024</v>
       </c>
-      <c r="E3" s="1">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1">
-        <v>138</v>
-      </c>
-      <c r="J3" s="1">
-        <v>7480201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2022</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="E15" s="4">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="1">
+        <v>138</v>
+      </c>
+      <c r="J15" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E16" s="4">
+        <v>39</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1">
+        <v>138</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="1">
-        <v>138</v>
-      </c>
-      <c r="J4" s="1">
-        <v>7480201</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="D17" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E17" s="4">
+        <v>42</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1">
+        <v>138</v>
+      </c>
+      <c r="J17" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2025</v>
-      </c>
-      <c r="E5" s="1">
-        <v>33</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1">
-        <v>138</v>
-      </c>
-      <c r="J5" s="1">
-        <v>7480201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2023</v>
-      </c>
-      <c r="E6" s="1">
-        <v>44</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="1">
-        <v>138</v>
-      </c>
-      <c r="J6" s="1">
-        <v>7480201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2024</v>
+      </c>
+      <c r="E18" s="4">
+        <v>43</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1">
+        <v>138</v>
+      </c>
+      <c r="J18" s="1">
+        <v>7480201</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
thêm file chitietphancong data excel
</commit_message>
<xml_diff>
--- a/Tài liệu/lop_data.xlsx
+++ b/Tài liệu/lop_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\NghienCuuKhoaHoc\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8205771F-A5EF-4156-80B1-5F2E58D3CD95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483E769C-6334-4841-ADF8-A5530FA65B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="81">
   <si>
     <t>MALOP</t>
   </si>
@@ -169,6 +169,105 @@
   </si>
   <si>
     <t>DA24TTC</t>
+  </si>
+  <si>
+    <t>Nhóm 1</t>
+  </si>
+  <si>
+    <t>Nhóm 2</t>
+  </si>
+  <si>
+    <t>Nhóm 3</t>
+  </si>
+  <si>
+    <t>Nhóm 4</t>
+  </si>
+  <si>
+    <t>Nhóm 5</t>
+  </si>
+  <si>
+    <t>Nhóm 6</t>
+  </si>
+  <si>
+    <t>Nhóm 7</t>
+  </si>
+  <si>
+    <t>Nhóm 8</t>
+  </si>
+  <si>
+    <t>Nhóm 9</t>
+  </si>
+  <si>
+    <t>Nhóm 10</t>
+  </si>
+  <si>
+    <t>Nhóm 11</t>
+  </si>
+  <si>
+    <t>Nhóm 12</t>
+  </si>
+  <si>
+    <t>Nhóm 13</t>
+  </si>
+  <si>
+    <t>Nhóm 14</t>
+  </si>
+  <si>
+    <t>Nhóm 15</t>
+  </si>
+  <si>
+    <t>Nhóm 16</t>
+  </si>
+  <si>
+    <t>Nhóm 17</t>
+  </si>
+  <si>
+    <t>Nhóm 18</t>
+  </si>
+  <si>
+    <t>Nhóm 19</t>
+  </si>
+  <si>
+    <t>Nhóm 20</t>
+  </si>
+  <si>
+    <t>Nhóm 21</t>
+  </si>
+  <si>
+    <t>Nhóm 22</t>
+  </si>
+  <si>
+    <t>Nhóm 23</t>
+  </si>
+  <si>
+    <t>Nhóm 24</t>
+  </si>
+  <si>
+    <t>Nhóm 25</t>
+  </si>
+  <si>
+    <t>Nhóm 26</t>
+  </si>
+  <si>
+    <t>Nhóm 27</t>
+  </si>
+  <si>
+    <t>Nhóm 28</t>
+  </si>
+  <si>
+    <t>Nhóm 29</t>
+  </si>
+  <si>
+    <t>Nhóm 30</t>
+  </si>
+  <si>
+    <t>Nhóm 31</t>
+  </si>
+  <si>
+    <t>Nhóm 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhóm 2 </t>
   </si>
 </sst>
 </file>
@@ -211,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,6 +333,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -247,10 +357,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -532,22 +642,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="33.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="24.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -582,7 +695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -595,7 +708,7 @@
       <c r="D2" s="1">
         <v>2020</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -614,7 +727,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -627,7 +740,7 @@
       <c r="D3" s="1">
         <v>2020</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>44</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -646,7 +759,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -659,7 +772,7 @@
       <c r="D4" s="1">
         <v>2021</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>44</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -678,7 +791,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -691,7 +804,7 @@
       <c r="D5" s="1">
         <v>2021</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -710,7 +823,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -723,7 +836,7 @@
       <c r="D6" s="1">
         <v>2021</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -742,7 +855,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -755,7 +868,7 @@
       <c r="D7" s="1">
         <v>2022</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -774,7 +887,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -787,7 +900,7 @@
       <c r="D8" s="1">
         <v>2022</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -806,7 +919,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -819,7 +932,7 @@
       <c r="D9" s="1">
         <v>2022</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -838,7 +951,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
@@ -851,7 +964,7 @@
       <c r="D10" s="1">
         <v>2022</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -870,7 +983,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -883,7 +996,7 @@
       <c r="D11" s="1">
         <v>2023</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -902,7 +1015,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -915,7 +1028,7 @@
       <c r="D12" s="1">
         <v>2023</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -934,7 +1047,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -947,7 +1060,7 @@
       <c r="D13" s="1">
         <v>2023</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>50</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -966,7 +1079,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -979,7 +1092,7 @@
       <c r="D14" s="1">
         <v>2023</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
@@ -998,7 +1111,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1011,7 +1124,7 @@
       <c r="D15" s="1">
         <v>2024</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -1030,7 +1143,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>46</v>
       </c>
@@ -1043,7 +1156,7 @@
       <c r="D16" s="1">
         <v>2024</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>39</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1062,7 +1175,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -1075,7 +1188,7 @@
       <c r="D17" s="1">
         <v>2024</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1094,7 +1207,7 @@
         <v>7480201</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1220,7 @@
       <c r="D18" s="1">
         <v>2024</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1123,6 +1236,1030 @@
         <v>138</v>
       </c>
       <c r="J18" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E19" s="4">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1">
+        <v>138</v>
+      </c>
+      <c r="J19" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="4">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1">
+        <v>138</v>
+      </c>
+      <c r="J20" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E21" s="4">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1">
+        <v>138</v>
+      </c>
+      <c r="J21" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E22" s="4">
+        <v>30</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1">
+        <v>138</v>
+      </c>
+      <c r="J22" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E23" s="4">
+        <v>30</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1">
+        <v>138</v>
+      </c>
+      <c r="J23" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E24" s="4">
+        <v>30</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="1">
+        <v>138</v>
+      </c>
+      <c r="J24" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E25" s="4">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1">
+        <v>138</v>
+      </c>
+      <c r="J25" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E26" s="4">
+        <v>30</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="1">
+        <v>138</v>
+      </c>
+      <c r="J26" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E27" s="4">
+        <v>30</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1">
+        <v>138</v>
+      </c>
+      <c r="J27" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E28" s="4">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="1">
+        <v>138</v>
+      </c>
+      <c r="J28" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E29" s="4">
+        <v>30</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="1">
+        <v>138</v>
+      </c>
+      <c r="J29" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E30" s="4">
+        <v>30</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1">
+        <v>138</v>
+      </c>
+      <c r="J30" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E31" s="4">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="1">
+        <v>138</v>
+      </c>
+      <c r="J31" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E32" s="4">
+        <v>30</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="1">
+        <v>138</v>
+      </c>
+      <c r="J32" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E33" s="4">
+        <v>30</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="1">
+        <v>138</v>
+      </c>
+      <c r="J33" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E34" s="4">
+        <v>30</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="1">
+        <v>138</v>
+      </c>
+      <c r="J34" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E35" s="4">
+        <v>30</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="1">
+        <v>138</v>
+      </c>
+      <c r="J35" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E36" s="4">
+        <v>30</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="1">
+        <v>138</v>
+      </c>
+      <c r="J36" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E37" s="4">
+        <v>30</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="1">
+        <v>138</v>
+      </c>
+      <c r="J37" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E38" s="4">
+        <v>30</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="1">
+        <v>138</v>
+      </c>
+      <c r="J38" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E39" s="4">
+        <v>30</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="1">
+        <v>138</v>
+      </c>
+      <c r="J39" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E40" s="4">
+        <v>30</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="1">
+        <v>138</v>
+      </c>
+      <c r="J40" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E41" s="4">
+        <v>30</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="1">
+        <v>138</v>
+      </c>
+      <c r="J41" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E42" s="4">
+        <v>30</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="1">
+        <v>138</v>
+      </c>
+      <c r="J42" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E43" s="4">
+        <v>30</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="1">
+        <v>138</v>
+      </c>
+      <c r="J43" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E44" s="4">
+        <v>30</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="1">
+        <v>138</v>
+      </c>
+      <c r="J44" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E45" s="4">
+        <v>30</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="1">
+        <v>138</v>
+      </c>
+      <c r="J45" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E46" s="4">
+        <v>30</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="1">
+        <v>138</v>
+      </c>
+      <c r="J46" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E47" s="4">
+        <v>30</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="1">
+        <v>138</v>
+      </c>
+      <c r="J47" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E48" s="4">
+        <v>30</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" s="1">
+        <v>138</v>
+      </c>
+      <c r="J48" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E49" s="4">
+        <v>30</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="1">
+        <v>138</v>
+      </c>
+      <c r="J49" s="1">
+        <v>7480201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E50" s="4">
+        <v>30</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="1">
+        <v>138</v>
+      </c>
+      <c r="J50" s="1">
         <v>7480201</v>
       </c>
     </row>

</xml_diff>